<commit_message>
Últimas modificaciones realizadas a Carga Masiva
</commit_message>
<xml_diff>
--- a/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
+++ b/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>TipoSolicitud</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>RutCliente</t>
+  </si>
+  <si>
+    <t>123A</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,10 +598,10 @@
     <col min="7" max="7" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="2" customWidth="1"/>
     <col min="14" max="14" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -664,8 +667,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>123</v>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Se mejora Carga Masiva y se perfecciona Internos
</commit_message>
<xml_diff>
--- a/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
+++ b/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
@@ -88,9 +88,6 @@
     <t>Cliente B</t>
   </si>
   <si>
-    <t>Ñuñoa</t>
-  </si>
-  <si>
     <t>23456789-0</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>RutCliente</t>
   </si>
   <si>
-    <t>123A</t>
-  </si>
-  <si>
     <t>14735905-5</t>
   </si>
   <si>
@@ -146,6 +140,12 @@
   </si>
   <si>
     <t>sin tono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    123A</t>
+  </si>
+  <si>
+    <t>chépica</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +633,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -651,25 +651,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>14</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -707,16 +707,16 @@
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>15</v>
@@ -739,19 +739,19 @@
         <v>123</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="R3" s="2">
         <v>8564789</v>
@@ -762,7 +762,7 @@
         <v>123</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -796,13 +796,13 @@
         <v>12</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Falta revisión por David
</commit_message>
<xml_diff>
--- a/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
+++ b/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>TipoSolicitud</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>sin tono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    123A</t>
   </si>
   <si>
     <t>chépica</t>
@@ -297,8 +294,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:A7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:A8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A8"/>
   <tableColumns count="1">
     <tableColumn id="1" name="NumeroSolicitud" dataDxfId="0"/>
   </tableColumns>
@@ -603,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,8 +685,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
+      <c r="A2" s="3">
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -770,7 +767,7 @@
         <v>456</v>
       </c>
       <c r="R5" s="2">
-        <v>6547895</v>
+        <v>6587945</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -799,7 +796,7 @@
         <v>23</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>21</v>
@@ -826,6 +823,11 @@
       </c>
       <c r="R7" s="2">
         <v>6547895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimos Arreglos realizados a Carga Masiva
</commit_message>
<xml_diff>
--- a/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
+++ b/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Mimet\MiLogistic\Despacho\3 - Proyecto\Despacho\WebApp\Content\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\David\Despacho\3 - Proyecto\Despacho\WebApp\Content\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F32A57C-16C0-435A-8246-B14E86273733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="+FT2744KSyqe7vmkdncBS5u1MGTHTzZZ42KPNki1qkXNRAJL3sEj0hcKtqv4VgYgJm2pvsKE++hhQaKStGPo2Q==" workbookSaltValue="u6TrE+AE+rS+Bi9xBE3B2w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="2415" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="2415" windowWidth="21600" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="CargaMasivaDetalle" sheetId="3" r:id="rId1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="414">
   <si>
     <t>TipoSolicitud</t>
   </si>
@@ -1247,12 +1246,48 @@
   </si>
   <si>
     <t>6547895</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>A1234</t>
+  </si>
+  <si>
+    <t>hoy</t>
+  </si>
+  <si>
+    <t>mañana</t>
+  </si>
+  <si>
+    <t>no me acuerdo</t>
+  </si>
+  <si>
+    <t>se me olvidó</t>
+  </si>
+  <si>
+    <t>que me voy a acordar</t>
+  </si>
+  <si>
+    <t>menos todavía</t>
+  </si>
+  <si>
+    <t>45789</t>
+  </si>
+  <si>
+    <t>2653</t>
+  </si>
+  <si>
+    <t>no interesa</t>
+  </si>
+  <si>
+    <t>256-8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1391,67 +1426,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FB5A9E34-9F91-48D9-BDCD-89FAB5ABD226}" name="Tabla4" displayName="Tabla4" ref="A1:R1562" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A1:R1562" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{31E491D5-5CAC-4651-8D9F-20BAA8C3ABA0}" name="NumeroSolicitud" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{B4A01A06-1D80-4898-97D7-8CBE2534853B}" name="TipoSolicitud" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3BBAD0EC-0A69-46F4-A6FA-8DA5E4C61080}" name="FechaSolicitud" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{A03C5CED-522A-484E-A023-1C50571A59C1}" name="FechaRecepcion" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{06588494-A2A1-4C1F-93BD-C4F969D31A2B}" name="NumeroCliente" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{06A1054C-892B-4E1B-9CA3-EA0BB86B6BF4}" name="NombreCliente" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{4AB43F41-CA43-43A7-953A-95DFE7C8B3EF}" name="CalleDireccionCliente" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{03E3D881-5E40-41AB-8D4E-0886EA2C1F33}" name="NumeroDireccionCliente" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{7B13279E-DECF-4C02-A2DC-CA8F2B9795B7}" name="RegionCliente" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{DDFF9974-D1C1-4996-96AC-49954150B93F}" name="ComunaCliente" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{FDBCF644-1328-42E5-871C-FBF5404F4648}" name="NumeroTelefonoContacto" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{6944327B-D692-42E6-9132-EC33F6213809}" name="NumeroTelefonoContactoAdicional" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{31E98D23-7B57-422A-AB80-8FFA0378792F}" name="RutCliente" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{9618FD29-F951-47BB-AEB8-ED0704F5ABAF}" name="UnidadNegocio" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{60D5F472-48C8-47B5-B7EF-292E1BA956D5}" name="Gerencia" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{DB3A4AFE-C572-4042-83D6-07AA8F6B0F5F}" name="ObservacionAof" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{6030BB0D-7DD6-4C8C-98D5-42A096A38E65}" name="Prioridad" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{B05B741D-917A-4F62-921C-986F94F056E1}" name="Placa" dataDxfId="0"/>
+    <tableColumn id="1" name="NumeroSolicitud" dataDxfId="17"/>
+    <tableColumn id="2" name="TipoSolicitud" dataDxfId="16"/>
+    <tableColumn id="3" name="FechaSolicitud" dataDxfId="15"/>
+    <tableColumn id="4" name="FechaRecepcion" dataDxfId="14"/>
+    <tableColumn id="5" name="NumeroCliente" dataDxfId="13"/>
+    <tableColumn id="6" name="NombreCliente" dataDxfId="12"/>
+    <tableColumn id="7" name="CalleDireccionCliente" dataDxfId="11"/>
+    <tableColumn id="8" name="NumeroDireccionCliente" dataDxfId="10"/>
+    <tableColumn id="9" name="RegionCliente" dataDxfId="9"/>
+    <tableColumn id="10" name="ComunaCliente" dataDxfId="8"/>
+    <tableColumn id="11" name="NumeroTelefonoContacto" dataDxfId="7"/>
+    <tableColumn id="12" name="NumeroTelefonoContactoAdicional" dataDxfId="6"/>
+    <tableColumn id="13" name="RutCliente" dataDxfId="5"/>
+    <tableColumn id="14" name="UnidadNegocio" dataDxfId="4"/>
+    <tableColumn id="15" name="Gerencia" dataDxfId="3"/>
+    <tableColumn id="16" name="ObservacionAof" dataDxfId="2"/>
+    <tableColumn id="17" name="Prioridad" dataDxfId="1"/>
+    <tableColumn id="18" name="Placa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla3" displayName="Tabla3" ref="B2:B7" totalsRowShown="0">
-  <autoFilter ref="B2:B7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B2:B7" totalsRowShown="0">
+  <autoFilter ref="B2:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TiposSolicitud"/>
+    <tableColumn id="1" name="TiposSolicitud"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC6A3BE6-0DD1-473A-8145-AE3E82651011}" name="Tabla1" displayName="Tabla1" ref="D2:D18" totalsRowShown="0">
-  <autoFilter ref="D2:D18" xr:uid="{68A12092-43EB-4139-ACED-88ED7DF53253}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="D2:D18" totalsRowShown="0">
+  <autoFilter ref="D2:D18"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B03C286A-C8EA-4272-B276-ECA431D2499B}" name="Regiones"/>
+    <tableColumn id="1" name="Regiones"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{299E1C2E-671D-498B-BFF4-F08F9FBEF802}" name="Tabla2" displayName="Tabla2" ref="F2:G348" totalsRowShown="0">
-  <autoFilter ref="F2:G348" xr:uid="{F4F113A8-EF3F-43C3-BC5F-CC50BB1BDAF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="F2:G348" totalsRowShown="0">
+  <autoFilter ref="F2:G348"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EAA0CC1E-25D8-47FA-ADAB-A4F43911C4A7}" name="Región"/>
-    <tableColumn id="2" xr3:uid="{A6273B29-6ACC-4CFF-AA93-3A51303CEC26}" name="Comuna"/>
+    <tableColumn id="1" name="Región"/>
+    <tableColumn id="2" name="Comuna"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{68705160-8C38-4266-91FB-1347CE9F1E9F}" name="Tabla5" displayName="Tabla5" ref="I2:I5" totalsRowShown="0">
-  <autoFilter ref="I2:I5" xr:uid="{604F318A-4D97-42C7-8E62-8D65944F26D4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="I2:I5" totalsRowShown="0">
+  <autoFilter ref="I2:I5"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2468C6EB-27D9-4F37-A7F7-E05497886F65}" name="Prioridad"/>
+    <tableColumn id="1" name="Prioridad"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1533,23 +1568,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1585,23 +1603,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1777,11 +1778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CBA57C-81D0-48AB-85C2-9B669FBF9B3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1562"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,8 +1863,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>123</v>
+      <c r="A2" s="2" t="s">
+        <v>403</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>33</v>
@@ -1916,28 +1917,52 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>123</v>
+      <c r="A3" s="2" t="s">
+        <v>402</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>413</v>
+      </c>
       <c r="N3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="2"/>
+      <c r="P3" s="2" t="s">
+        <v>412</v>
+      </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2">
         <v>8564789</v>
@@ -33169,7 +33194,7 @@
     <protectedRange sqref="A2:R1048576" name="Tabla"/>
   </protectedRanges>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J1562" xr:uid="{A9C5A567-C67C-4D6C-8D2C-0999D06F02D5}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J1562">
       <formula1>INDIRECT($I$2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -33181,19 +33206,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{6B9063E6-ACD9-4F95-84A4-49B908865474}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$B$3:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1562</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1F53A705-ECB7-4FD9-B4B3-6925B482ABED}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$D$3:$D$18</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1562</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F17006D2-8C1E-4153-B4FF-AE6505984448}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$I$3:$I$5</xm:f>
           </x14:formula1>
@@ -33206,7 +33231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I348"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">

</xml_diff>

<commit_message>
Validaciones en Servidor Listas
</commit_message>
<xml_diff>
--- a/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
+++ b/3 - Proyecto/Despacho/WebApp/Content/Archivos/Carga Masiva.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="414">
   <si>
     <t>TipoSolicitud</t>
   </si>
@@ -1781,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,9 +1890,7 @@
       <c r="I2" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
         <v>400</v>
       </c>
@@ -1979,8 +1977,12 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -2076,7 +2078,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>

</xml_diff>